<commit_message>
attempting manual sql queries
</commit_message>
<xml_diff>
--- a/test/testcases/testcase28_manual_sql_etltesting.xlsx
+++ b/test/testcases/testcase28_manual_sql_etltesting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\QE_ATF\test\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B90097A-7ADE-42E4-8AB8-6469EC9A8AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A77AF6-D1C7-4BCC-ACE0-31B58A0800C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testcase" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>sourcequerymode</t>
   </si>
@@ -165,19 +165,13 @@
     <t>id</t>
   </si>
   <si>
-    <t>s2tcompare</t>
-  </si>
-  <si>
-    <t>/app/test/s2t/s2t_28_oracle_manual_query.xlsx</t>
-  </si>
-  <si>
-    <t>source_to_target</t>
-  </si>
-  <si>
     <t>/app/test/sql/sourcesql</t>
   </si>
   <si>
     <t>/app/test/sql/targetsql</t>
+  </si>
+  <si>
+    <t>likeobjectcompare</t>
   </si>
 </sst>
 </file>
@@ -572,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +591,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -694,7 +688,7 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -790,7 +784,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -805,17 +799,13 @@
       <c r="A30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="B30" s="3"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="B31" s="3"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">

</xml_diff>